<commit_message>
Add link to astro SIMS
</commit_message>
<xml_diff>
--- a/CourseDocs/ExtraResources.xlsx
+++ b/CourseDocs/ExtraResources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Documents\Astronomy\CourseDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7034B5E6-5ACD-4A22-A63B-E3E275CA751B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC0DA9A-A973-4EAE-947F-494571313D74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" activeTab="2" xr2:uid="{4E8BF544-0EF5-4BE7-85EF-9A39667A5938}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
   <si>
     <t>Source</t>
   </si>
@@ -304,6 +304,15 @@
   </si>
   <si>
     <t>https://www.jpl.nasa.gov/edu/learn/project/explore-earth-and-space-with-art/</t>
+  </si>
+  <si>
+    <t>SIMULATION LIST</t>
+  </si>
+  <si>
+    <t>List of HTML, Native, and Java Astro SIMS</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1UN2LIh8TIoAYmp20fA9wYNC4XeJsuFte7fp4hPGfrMI/edit#gid=0</t>
   </si>
 </sst>
 </file>
@@ -905,10 +914,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC74960-B8A0-4065-A010-82787F36C067}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1044,6 +1053,17 @@
         <v>88</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{58FB2B02-9E58-42C4-9B55-1C47044E51EF}"/>
@@ -1055,6 +1075,7 @@
     <hyperlink ref="E8" r:id="rId7" xr:uid="{8CF68DBD-D38D-4904-9C12-D13A3B651959}"/>
     <hyperlink ref="E9" r:id="rId8" xr:uid="{329AAF0A-A0F1-42B6-B9E8-9A48F07D8DE9}"/>
     <hyperlink ref="E10" r:id="rId9" xr:uid="{2AFA9BEB-8FF3-40FE-A410-FAE4028EA24A}"/>
+    <hyperlink ref="E11" r:id="rId10" location="gid=0" xr:uid="{78630DBE-832D-455B-B69D-99D2D85880B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>